<commit_message>
Added the batch number column
Added the batch number column to Redeemed Gifts Report
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateRedeemedGifts.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateRedeemedGifts.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6945C976-7736-4BBD-A297-116EB6A231B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="-150" windowWidth="28710" windowHeight="5955" activeTab="1"/>
+    <workbookView xWindow="-24120" yWindow="1095" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RedeemedGifts" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Contact Date</t>
   </si>
@@ -81,12 +87,15 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Batch Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,19 +239,22 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -255,15 +267,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -279,14 +288,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -324,7 +336,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -396,7 +408,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -569,7 +581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -592,27 +604,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -674,11 +686,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -693,10 +705,11 @@
     <col min="9" max="9" width="86.85546875" style="7" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" style="7" customWidth="1"/>
     <col min="11" max="11" width="48.28515625" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="7"/>
+    <col min="12" max="12" width="34.28515625" style="7" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -724,14 +737,17 @@
       <c r="I1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="16" t="s">
         <v>21</v>
       </c>
+      <c r="L1" s="16" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -743,11 +759,12 @@
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -761,10 +778,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Please choose option from Dropdown list" promptTitle="Make Selection" sqref="F1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Please choose option from Dropdown list" promptTitle="Make Selection" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Option 3 (Perfume Set), Option 1 (Firming-up Gel), Option 2 (Face Wash &amp; Day Moisturiser)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Make Selection" prompt="Please select &quot;Yes&quot; or &quot;no&quot;" sqref="G1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Make Selection" prompt="Please select &quot;Yes&quot; or &quot;no&quot;" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>